<commit_message>
Criação de Placas pra Fita Borda
</commit_message>
<xml_diff>
--- a/layout_fita.xlsx
+++ b/layout_fita.xlsx
@@ -15,14 +15,14 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$B$4</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$B$5</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>PRODUTO</t>
   </si>
@@ -35,12 +35,15 @@
   <si>
     <t xml:space="preserve">IDENTIFICAÇÃO DE MATERIAIS </t>
   </si>
+  <si>
+    <t>COR</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -64,7 +67,13 @@
     </font>
     <font>
       <b/>
-      <sz val="30"/>
+      <sz val="28"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="24"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -128,7 +137,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
@@ -139,6 +148,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
   </cellXfs>
@@ -484,7 +496,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
@@ -502,23 +514,29 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="236.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="5" t="s">
+    <row r="2" spans="1:2" ht="120" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="6" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="1"/>
     </row>
-    <row r="3" spans="1:2" ht="236.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="3" t="s">
-        <v>1</v>
+    <row r="3" spans="1:2" ht="138.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="5" t="s">
+        <v>4</v>
       </c>
       <c r="B3" s="1"/>
     </row>
-    <row r="4" spans="1:2" ht="236.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" ht="225" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="1"/>
+    </row>
+    <row r="5" spans="1:2" ht="236.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="1"/>
+      <c r="B5" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>